<commit_message>
Working on chapter 4.
</commit_message>
<xml_diff>
--- a/speakur-components.xlsx
+++ b/speakur-components.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Function</t>
   </si>
@@ -192,6 +192,63 @@
   </si>
   <si>
     <t>Element wrapper around i18next library</t>
+  </si>
+  <si>
+    <t>Database tables</t>
+  </si>
+  <si>
+    <t>admins</t>
+  </si>
+  <si>
+    <t>posts</t>
+  </si>
+  <si>
+    <t>$uid</t>
+  </si>
+  <si>
+    <t>$parent-&gt;$child</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>author, text, replyTo, threadId, timestamp</t>
+  </si>
+  <si>
+    <t>table name</t>
+  </si>
+  <si>
+    <t>key structure</t>
+  </si>
+  <si>
+    <t>notable fields</t>
+  </si>
+  <si>
+    <t>postvotes</t>
+  </si>
+  <si>
+    <t>up,down,timestamp</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>threads</t>
+  </si>
+  <si>
+    <t>$threadId</t>
+  </si>
+  <si>
+    <t>uservotes</t>
+  </si>
+  <si>
+    <t>$uid-&gt;$parent-$child</t>
+  </si>
+  <si>
+    <t>uid, username, email, picture_link</t>
+  </si>
+  <si>
+    <t>owner, created, title, href, allowAnonymous</t>
   </si>
 </sst>
 </file>
@@ -509,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -765,6 +822,88 @@
         <v>54</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chapter 4 pretty much done.
</commit_message>
<xml_diff>
--- a/speakur-components.xlsx
+++ b/speakur-components.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
   <si>
     <t>Function</t>
   </si>
@@ -249,6 +249,60 @@
   </si>
   <si>
     <t>owner, created, title, href, allowAnonymous</t>
+  </si>
+  <si>
+    <t>Load times - Opera, Windows 7, cache disabled</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Production (Vulcanized)</t>
+  </si>
+  <si>
+    <t>Time to load</t>
+  </si>
+  <si>
+    <t>Time to display 25 comments</t>
+  </si>
+  <si>
+    <t>2800 ms</t>
+  </si>
+  <si>
+    <t>~7000ms</t>
+  </si>
+  <si>
+    <t>1100 ms</t>
+  </si>
+  <si>
+    <t>Google Chrome</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Vulcanized</t>
+  </si>
+  <si>
+    <t>2200 ms</t>
+  </si>
+  <si>
+    <t>4200 ms</t>
+  </si>
+  <si>
+    <t>1150 ms</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>7400 ms</t>
+  </si>
+  <si>
+    <t>6050 ms</t>
+  </si>
+  <si>
+    <t>2900 ms</t>
   </si>
 </sst>
 </file>
@@ -566,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -904,6 +958,95 @@
         <v>67</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42">
+        <v>10500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished ch. 5 and general cleanup for first complete draft.
</commit_message>
<xml_diff>
--- a/speakur-components.xlsx
+++ b/speakur-components.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
   <si>
     <t>Function</t>
   </si>
@@ -254,27 +254,6 @@
     <t>Load times - Opera, Windows 7, cache disabled</t>
   </si>
   <si>
-    <t>Development</t>
-  </si>
-  <si>
-    <t>Production (Vulcanized)</t>
-  </si>
-  <si>
-    <t>Time to load</t>
-  </si>
-  <si>
-    <t>Time to display 25 comments</t>
-  </si>
-  <si>
-    <t>2800 ms</t>
-  </si>
-  <si>
-    <t>~7000ms</t>
-  </si>
-  <si>
-    <t>1100 ms</t>
-  </si>
-  <si>
     <t>Google Chrome</t>
   </si>
   <si>
@@ -284,25 +263,19 @@
     <t>Vulcanized</t>
   </si>
   <si>
-    <t>2200 ms</t>
-  </si>
-  <si>
-    <t>4200 ms</t>
-  </si>
-  <si>
-    <t>1150 ms</t>
-  </si>
-  <si>
     <t>Firefox</t>
   </si>
   <si>
-    <t>7400 ms</t>
-  </si>
-  <si>
-    <t>6050 ms</t>
-  </si>
-  <si>
-    <t>2900 ms</t>
+    <t>Initiatl</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Rate of Reduction</t>
   </si>
 </sst>
 </file>
@@ -338,8 +311,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +597,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -965,89 +939,125 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
         <v>78</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33">
+        <v>2800</v>
+      </c>
+      <c r="C33">
+        <v>1100</v>
+      </c>
+      <c r="D33" s="1">
+        <f>(C33-B33)/B33</f>
+        <v>-0.6071428571428571</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34">
+        <v>7000</v>
+      </c>
+      <c r="C34">
+        <v>2800</v>
+      </c>
+      <c r="D34" s="1">
+        <f>(C34-B34)/B34</f>
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37">
+        <v>2200</v>
+      </c>
+      <c r="C37">
+        <v>1150</v>
+      </c>
+      <c r="D37" s="1">
+        <f>(C37-B37)/B37</f>
+        <v>-0.47727272727272729</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38">
+        <v>4200</v>
+      </c>
+      <c r="C38">
+        <v>2900</v>
+      </c>
+      <c r="D38" s="1">
+        <f>(C38-B38)/B38</f>
+        <v>-0.30952380952380953</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41">
+        <v>7400</v>
+      </c>
+      <c r="C41">
+        <v>6050</v>
+      </c>
+      <c r="D41" s="1">
+        <f>(C41-B41)/B41</f>
+        <v>-0.18243243243243243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41">
+      <c r="B42">
         <v>12000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>91</v>
       </c>
       <c r="C42">
         <v>10500</v>
       </c>
+      <c r="D42" s="1">
+        <f>(C42-B42)/B42</f>
+        <v>-0.125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>